<commit_message>
New data and addition of the humanizer
</commit_message>
<xml_diff>
--- a/countries/Argentina.xlsx
+++ b/countries/Argentina.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/countries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/a-place-for-salvador-allende/countries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_037960F4F5CB49A86F9372B95981124C78C6AF50" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E77B7B8-0FFB-4153-BB8A-431D02D5D32A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_037960F4F5CB49A86F9372B95981124C78C6AF50" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EA17278-8FFC-43D1-B935-4F78B267C9A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>